<commit_message>
Fixed import and export
</commit_message>
<xml_diff>
--- a/src/main/java/org/openepics/names/ui/devices/NamingImportTemplate.xlsx
+++ b/src/main/java/org/openepics/names/ui/devices/NamingImportTemplate.xlsx
@@ -83,9 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,34 +427,35 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="22.125" customWidth="1"/>
-    <col min="5" max="5" width="26.375" customWidth="1"/>
-    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="1" max="2" width="11" style="3"/>
+    <col min="3" max="3" width="10.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -461,6 +464,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>